<commit_message>
update with dbo changes
</commit_message>
<xml_diff>
--- a/bos-onboarding/test/darshan_test.xlsx
+++ b/bos-onboarding/test/darshan_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\build2auto\bos-tools\bos-onboarding\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005A730A-7F4A-44A2-B854-97F3AC84115D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E09C19-CB5C-475E-A23A-89E05AEEB74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
   <si>
     <t>dbo.section</t>
   </si>
@@ -72,9 +72,6 @@
     <t>a388563d-58e3-4534-b133-19389f6650a4</t>
   </si>
   <si>
-    <t>UK-LON-KGX1</t>
-  </si>
-  <si>
     <t>Rooms</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>b9f2c8b8-d67e-4b50-824a-7b48ff877429</t>
   </si>
   <si>
-    <t>UK-LON-BLDNG1-FL1</t>
-  </si>
-  <si>
     <t>Zones</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
   </si>
   <si>
     <t>a0f68db4-f074-49cf-8e80-d65634587f9f</t>
-  </si>
-  <si>
-    <t>UK-LON-BLDNG1-RM1</t>
   </si>
   <si>
     <t>UK-LON-BLDNG1_RM2</t>
@@ -346,6 +337,30 @@
   </si>
   <si>
     <t>MV23</t>
+  </si>
+  <si>
+    <t>ELECTRICAL/CB_SS</t>
+  </si>
+  <si>
+    <t>ELECTRICAL/CB_SH</t>
+  </si>
+  <si>
+    <t>ELECTRICAL/CB_SJ</t>
+  </si>
+  <si>
+    <t>9e7c08d9-5c7b-47c7-a664-9e01cb070d31</t>
+  </si>
+  <si>
+    <t>9e7c08d9-5c7b-47c7-a664-9e01cb070d40</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>PQR</t>
+  </si>
+  <si>
+    <t>1=ON 0=OFF</t>
   </si>
 </sst>
 </file>
@@ -675,9 +690,9 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -734,55 +749,55 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>10</v>
@@ -790,19 +805,19 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1"/>
@@ -1811,9 +1826,9 @@
   </sheetPr>
   <dimension ref="A1:AD1003"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q3" sqref="Q3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -1844,79 +1859,79 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>85</v>
+      <c r="G1" s="1" t="s">
+        <v>80</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
+      <c r="H1" s="10" t="s">
+        <v>83</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>83</v>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>86</v>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="Z1" s="4"/>
       <c r="AA1" s="4"/>
@@ -1926,63 +1941,65 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q2" s="3">
         <v>112345</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
-      <c r="S2" s="3"/>
+      <c r="S2" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
@@ -1992,65 +2009,67 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q3" s="3">
         <v>1123457</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
-      <c r="S3" s="3"/>
+      <c r="S3" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
@@ -2060,63 +2079,65 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q4" s="3">
         <v>1123456</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
-      <c r="S4" s="3"/>
+      <c r="S4" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
@@ -34112,9 +34133,9 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -34132,65 +34153,73 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>39</v>
+      <c r="G1" s="1" t="s">
+        <v>52</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>103</v>
+      <c r="E2" s="3" t="s">
+        <v>109</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>101</v>
+      <c r="F2" s="3" t="s">
+        <v>107</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>104</v>
+      <c r="E3" s="3" t="s">
+        <v>109</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>102</v>
+      <c r="F3" s="3" t="s">
+        <v>108</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -34996,7 +35025,7 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I76" s="4"/>
     </row>
@@ -35020,7 +35049,7 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I78" s="4"/>
     </row>
@@ -35253,7 +35282,7 @@
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I99" s="4"/>
     </row>
@@ -35266,7 +35295,7 @@
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I100" s="4"/>
     </row>
@@ -35510,10 +35539,10 @@
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
       <c r="H122" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="15.75" customHeight="1">
@@ -35525,10 +35554,10 @@
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="15.75" customHeight="1">
@@ -35541,7 +35570,7 @@
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
       <c r="I124" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="15.75" customHeight="1">
@@ -35553,10 +35582,10 @@
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="15.75" customHeight="1">
@@ -35569,7 +35598,7 @@
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15.75" customHeight="1">
@@ -35581,10 +35610,10 @@
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
       <c r="H127" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="15.75" customHeight="1">
@@ -35597,7 +35626,7 @@
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="15.75" customHeight="1">
@@ -35610,7 +35639,7 @@
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="15.75" customHeight="1">
@@ -35623,7 +35652,7 @@
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="15.75" customHeight="1">
@@ -35635,10 +35664,10 @@
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
       <c r="H131" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="15.75" customHeight="1">
@@ -35651,7 +35680,7 @@
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="15.75" customHeight="1">
@@ -35664,7 +35693,7 @@
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="15.75" customHeight="1">
@@ -35677,7 +35706,7 @@
       <c r="G134" s="3"/>
       <c r="H134" s="3"/>
       <c r="I134" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="15.75" customHeight="1">
@@ -35690,7 +35719,7 @@
       <c r="G135" s="3"/>
       <c r="H135" s="3"/>
       <c r="I135" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="15.75" customHeight="1">
@@ -35703,7 +35732,7 @@
       <c r="G136" s="3"/>
       <c r="H136" s="3"/>
       <c r="I136" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="15.75" customHeight="1">
@@ -35716,7 +35745,7 @@
       <c r="G137" s="3"/>
       <c r="H137" s="3"/>
       <c r="I137" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="15.75" customHeight="1">
@@ -35751,7 +35780,7 @@
       <c r="G140" s="3"/>
       <c r="H140" s="3"/>
       <c r="I140" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="15.75" customHeight="1">
@@ -35961,10 +35990,10 @@
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
       <c r="H159" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="15.75" customHeight="1">
@@ -35977,7 +36006,7 @@
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
       <c r="I160" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="161" ht="15.75" customHeight="1"/>
@@ -36835,7 +36864,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -36850,19 +36879,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
@@ -38694,7 +38723,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -38708,61 +38737,61 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
rooms, zone - connections, multiple values accept
</commit_message>
<xml_diff>
--- a/bos-onboarding/test/darshan_test.xlsx
+++ b/bos-onboarding/test/darshan_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\build2auto\bos-tools\bos-onboarding\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E09C19-CB5C-475E-A23A-89E05AEEB74E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821F7403-71C9-4890-9751-E809F359CCD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
   <si>
     <t>dbo.section</t>
   </si>
@@ -361,6 +361,18 @@
   </si>
   <si>
     <t>1=ON 0=OFF</t>
+  </si>
+  <si>
+    <t>UK-LON-BLDNG1_FL1,UK-LON-BLDNG1</t>
+  </si>
+  <si>
+    <t>UK-LON-BLDNG1_RM1,UK-LON-BLDNG1_FL1,UK-LON-BLDNG1</t>
+  </si>
+  <si>
+    <t>UK-LON-BLDNG1_RM2,UK-LON-BLDNG1_FL1,UK-LON-BLDNG1</t>
+  </si>
+  <si>
+    <t>UK-LON-BLDNG1,UK-LON-BLDNG1_FL1</t>
   </si>
 </sst>
 </file>
@@ -692,7 +704,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -766,7 +778,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
@@ -783,7 +795,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
@@ -800,7 +812,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1">
@@ -817,7 +829,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
device connections and cloud device id code added
</commit_message>
<xml_diff>
--- a/bos-onboarding/test/darshan_test.xlsx
+++ b/bos-onboarding/test/darshan_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\build2auto\bos-tools\bos-onboarding\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821F7403-71C9-4890-9751-E809F359CCD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2237BCD1-A466-4B16-A89D-21398ADCF676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="asset_template" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">assets!$A$1:$Y$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">assets!$A$1:$Z$4</definedName>
     <definedName name="Z_AA0593A2_B62E_4E85_A9F1_4940BAB73F65_.wvu.FilterData" localSheetId="1" hidden="1">assets!$A$1:$Y$23</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="112">
   <si>
     <t>dbo.section</t>
   </si>
@@ -261,9 +261,6 @@
     <t>IN-BLR-RIO</t>
   </si>
   <si>
-    <t>IN-BLR-RIO-7F-RM-1</t>
-  </si>
-  <si>
     <t>9e7c08d9-5c7b-47c7-a664-9e01cb070d39</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
   </si>
   <si>
     <t>AHU-102</t>
-  </si>
-  <si>
-    <t>IN-BLR-RIO-7F-RM-2</t>
   </si>
   <si>
     <t>PROXIED</t>
@@ -354,12 +348,6 @@
     <t>9e7c08d9-5c7b-47c7-a664-9e01cb070d40</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>PQR</t>
-  </si>
-  <si>
     <t>1=ON 0=OFF</t>
   </si>
   <si>
@@ -373,6 +361,12 @@
   </si>
   <si>
     <t>UK-LON-BLDNG1,UK-LON-BLDNG1_FL1</t>
+  </si>
+  <si>
+    <t>dbo.cloud_device_id</t>
+  </si>
+  <si>
+    <t>run_status</t>
   </si>
 </sst>
 </file>
@@ -702,9 +696,9 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B7"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -778,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
@@ -795,7 +789,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
@@ -812,7 +806,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1">
@@ -829,7 +823,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1"/>
@@ -1838,9 +1832,9 @@
   </sheetPr>
   <dimension ref="A1:AD1003"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -1877,7 +1871,7 @@
         <v>26</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>27</v>
@@ -1889,13 +1883,13 @@
         <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>31</v>
@@ -1919,7 +1913,7 @@
         <v>37</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>38</v>
@@ -1945,7 +1939,9 @@
       <c r="Y1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="4"/>
+      <c r="Z1" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
@@ -1968,19 +1964,19 @@
         <v>75</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>75</v>
@@ -1989,10 +1985,10 @@
         <v>72</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q2" s="3">
         <v>112345</v>
@@ -2001,7 +1997,7 @@
         <v>45</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
@@ -2013,7 +2009,9 @@
       <c r="Y2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="4"/>
+      <c r="Z2" s="4">
+        <v>1234</v>
+      </c>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
@@ -2021,7 +2019,7 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>73</v>
@@ -2036,33 +2034,33 @@
         <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>75</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="3">
         <v>1123457</v>
@@ -2071,7 +2069,7 @@
         <v>45</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -2083,7 +2081,9 @@
       <c r="Y3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Z3" s="4"/>
+      <c r="Z3" s="4">
+        <v>4567</v>
+      </c>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>73</v>
@@ -2106,31 +2106,31 @@
         <v>75</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>75</v>
       </c>
       <c r="N4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="P4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q4" s="3">
         <v>1123456</v>
@@ -2139,7 +2139,7 @@
         <v>45</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
@@ -2151,7 +2151,9 @@
       <c r="Y4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="4"/>
+      <c r="Z4" s="4">
+        <v>8910</v>
+      </c>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
@@ -34126,7 +34128,7 @@
       <c r="AD1003" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y23" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:Z4" xr:uid="{C8889A15-25B0-4577-9314-E9CD7C9CDFE3}"/>
   <customSheetViews>
     <customSheetView guid="{AA0593A2-B62E-4E85-A9F1-4940BAB73F65}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34145,7 +34147,7 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2:E3"/>
     </sheetView>
@@ -34171,7 +34173,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>49</v>
@@ -34192,22 +34194,22 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="4"/>
@@ -34215,22 +34217,22 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>

</xml_diff>

<commit_message>
feed and controls update with code
</commit_message>
<xml_diff>
--- a/bos-onboarding/test/darshan_test.xlsx
+++ b/bos-onboarding/test/darshan_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\build2auto\bos-tools\bos-onboarding\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2237BCD1-A466-4B16-A89D-21398ADCF676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C7AFF-EF99-47CA-A631-429DFBCD76AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
   <si>
     <t>dbo.section</t>
   </si>
@@ -366,7 +366,25 @@
     <t>dbo.cloud_device_id</t>
   </si>
   <si>
-    <t>run_status</t>
+    <t>volts: volts</t>
+  </si>
+  <si>
+    <t>VAV-102</t>
+  </si>
+  <si>
+    <t>9e7c08d9-5c7b-47c7-a664-9e01cb070d99</t>
+  </si>
+  <si>
+    <t>VAV_102</t>
+  </si>
+  <si>
+    <t>HVAC/VAV_SD_CSP</t>
+  </si>
+  <si>
+    <t>supplier_air_temperature_sensor</t>
+  </si>
+  <si>
+    <t>degrees_celcius: degrees_celcius</t>
   </si>
 </sst>
 </file>
@@ -459,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -476,6 +494,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1832,9 +1851,9 @@
   </sheetPr>
   <dimension ref="A1:AD1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -2142,7 +2161,9 @@
         <v>102</v>
       </c>
       <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
+      <c r="U4" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3" t="s">
@@ -2160,26 +2181,56 @@
       <c r="AD4" s="4"/>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="A5" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="11"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="4"/>
+      <c r="Q5" s="3">
+        <v>1234</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="U5" s="4"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
@@ -34149,7 +34200,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E3"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -34205,13 +34256,13 @@
       <c r="D2" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>105</v>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>93</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="3"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
@@ -34232,20 +34283,32 @@
         <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>

</xml_diff>

<commit_message>
workaround for backslash coming for double quotes
</commit_message>
<xml_diff>
--- a/bos-onboarding/test/darshan_test.xlsx
+++ b/bos-onboarding/test/darshan_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\build2auto\bos-tools\bos-onboarding\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C7AFF-EF99-47CA-A631-429DFBCD76AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C4F1C6-AC09-492C-9AAA-92560F8536EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="120">
   <si>
     <t>dbo.section</t>
   </si>
@@ -288,9 +288,6 @@
     <t>HLI-234</t>
   </si>
   <si>
-    <t>AHU-123, AHU-122</t>
-  </si>
-  <si>
     <t>udmi.bacnet_addr</t>
   </si>
   <si>
@@ -357,12 +354,6 @@
     <t>UK-LON-BLDNG1_RM1,UK-LON-BLDNG1_FL1,UK-LON-BLDNG1</t>
   </si>
   <si>
-    <t>UK-LON-BLDNG1_RM2,UK-LON-BLDNG1_FL1,UK-LON-BLDNG1</t>
-  </si>
-  <si>
-    <t>UK-LON-BLDNG1,UK-LON-BLDNG1_FL1</t>
-  </si>
-  <si>
     <t>dbo.cloud_device_id</t>
   </si>
   <si>
@@ -385,6 +376,21 @@
   </si>
   <si>
     <t>degrees_celcius: degrees_celcius</t>
+  </si>
+  <si>
+    <t>UK-LON-BLDNG1, UK-LON-BLDNG1_FL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UK-LON-BLDNG1_RM2, UK-LON-BLDNG1_FL1, UK-LON-BLDNG1</t>
+  </si>
+  <si>
+    <t>UK-LON-BLDNG2</t>
+  </si>
+  <si>
+    <t>AHU-123,AHU-122</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UK-LON-BLDNG1_RM2</t>
   </si>
 </sst>
 </file>
@@ -715,9 +721,9 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -774,7 +780,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
@@ -791,7 +797,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
@@ -808,7 +814,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
@@ -825,7 +831,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1">
@@ -842,7 +848,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1"/>
@@ -1851,9 +1857,9 @@
   </sheetPr>
   <dimension ref="A1:AD1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -1932,7 +1938,7 @@
         <v>37</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>38</v>
@@ -1959,7 +1965,7 @@
         <v>44</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
@@ -1982,15 +1988,13 @@
       <c r="E2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
         <v>80</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -2016,7 +2020,7 @@
         <v>45</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
@@ -2038,7 +2042,7 @@
     </row>
     <row r="3" spans="1:30" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>73</v>
@@ -2053,30 +2057,28 @@
         <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="I3" s="11"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>75</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>77</v>
@@ -2088,7 +2090,7 @@
         <v>45</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -2110,7 +2112,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>73</v>
@@ -2125,28 +2127,26 @@
         <v>75</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="11" t="s">
-        <v>85</v>
-      </c>
+      <c r="I4" s="11"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>75</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>77</v>
@@ -2158,7 +2158,7 @@
         <v>45</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3" t="s">
@@ -2182,7 +2182,7 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>73</v>
@@ -2197,26 +2197,26 @@
         <v>75</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="11"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>75</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3">
@@ -2226,10 +2226,10 @@
         <v>45</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U5" s="4"/>
       <c r="V5" s="3"/>
@@ -34224,7 +34224,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>49</v>
@@ -34245,45 +34245,45 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>
@@ -34291,23 +34291,23 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>

</xml_diff>